<commit_message>
ospi bra e feltre
</commit_message>
<xml_diff>
--- a/Copy of coordinate_stazioni.xlsx
+++ b/Copy of coordinate_stazioni.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipg-my.sharepoint.com/personal/vitoantonio_giannuzzi_dottorandi_unipg_it/Documents/PhD Agricolus/Agricolus/ConfrontoDatiMeteo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{2D15C3BC-2DAC-402E-9BCC-66C6650FED37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A8B9320-5980-4BCB-A33E-94F0BE37E3C4}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{2D15C3BC-2DAC-402E-9BCC-66C6650FED37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F16188C5-F74A-445B-9B34-4B121036F016}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Latitudine</t>
   </si>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,7 +424,7 @@
     <col min="3" max="3" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -435,7 +435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>7.8550000000000004</v>
       </c>
@@ -448,8 +448,11 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>11.61</v>
       </c>
@@ -462,8 +465,11 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>11.147</v>
       </c>
@@ -474,7 +480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11.907</v>
       </c>
@@ -488,7 +494,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>7.9880000000000004</v>
       </c>
@@ -499,7 +505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>12.10134</v>
       </c>
@@ -513,7 +519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>11.844030999999999</v>
       </c>
@@ -527,7 +533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>10.648</v>
       </c>
@@ -541,7 +547,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>12.26505</v>
       </c>
@@ -555,7 +561,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8.1342099999999995</v>
       </c>
@@ -569,7 +575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11.045</v>
       </c>
@@ -583,7 +589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cenesi e fosso ghiaia
</commit_message>
<xml_diff>
--- a/Copy of coordinate_stazioni.xlsx
+++ b/Copy of coordinate_stazioni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipg-my.sharepoint.com/personal/vitoantonio_giannuzzi_dottorandi_unipg_it/Documents/PhD Agricolus/Agricolus/ConfrontoDatiMeteo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{2D15C3BC-2DAC-402E-9BCC-66C6650FED37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCE96F91-2A3F-439E-9E79-56A0A8BE96CC}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{2D15C3BC-2DAC-402E-9BCC-66C6650FED37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FEFEC4C-7225-4DBE-A57D-2F94321B2B74}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Latitudine</t>
   </si>
@@ -414,7 +414,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,6 +566,9 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">

</xml_diff>